<commit_message>
master: fixed time estimation graph
</commit_message>
<xml_diff>
--- a/docs/project_management/time_estimation/time_estimation.xlsx
+++ b/docs/project_management/time_estimation/time_estimation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sap-my.sharepoint.com/personal/felix_hausberger_sap_com/Documents/Workspaces/IdeaProjects/dashup/docs/project_management/time_estimation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D070497\OneDrive - SAP SE\Workspaces\IdeaProjects\dashup\docs\project_management\time_estimation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{38D201AD-A7A5-43E4-9BB3-0ED51C1379B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{3C38BA63-706F-4ED8-AA96-7725E394D489}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="8_{38D201AD-A7A5-43E4-9BB3-0ED51C1379B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{957040BF-1B48-433F-A203-EEB4A582B69C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{70860DB2-D251-46E3-A3E4-9E8731226EC1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" xr2:uid="{70860DB2-D251-46E3-A3E4-9E8731226EC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -151,6 +151,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Time Estimation</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -211,6 +236,76 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:noFill/>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:trendline>
             <c:spPr>
               <a:ln w="19050" cap="rnd">
@@ -222,13 +317,14 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="7.4974190726159226E-2"/>
-                  <c:y val="-0.29351560221638962"/>
+                  <c:x val="5.3274278215223202E-2"/>
+                  <c:y val="-0.18262800149190386"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -311,8 +407,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -342,6 +439,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Estimated Time In Hours</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -365,6 +517,9 @@
           <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -404,6 +559,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Function</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Points</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1393,23 +1608,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88474A7B-6DD3-422E-8062-2B1A433E6E68}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -1417,7 +1632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1428,7 +1643,7 @@
         <v>16.72</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1439,7 +1654,7 @@
         <v>55.59</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1450,7 +1665,7 @@
         <v>59.84</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1461,12 +1676,16 @@
         <v>36.06</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9" s="2"/>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="17" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>11</v>
       </c>
@@ -1474,37 +1693,37 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>7</v>
       </c>
       <c r="B20" s="2">
-        <f>0.5087*C20+32.991</f>
-        <v>56.706593999999996</v>
+        <f>1.6551*C20</f>
+        <v>77.160761999999991</v>
       </c>
       <c r="C20" s="3">
         <v>46.62</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>8</v>
       </c>
       <c r="B21" s="2">
-        <f t="shared" ref="B21:B22" si="0">0.5087*C21+32.991</f>
-        <v>57.215294</v>
+        <f t="shared" ref="B21:B22" si="0">1.6551*C21</f>
+        <v>78.815861999999996</v>
       </c>
       <c r="C21" s="3">
         <v>47.62</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>4</v>
       </c>
       <c r="B22" s="2">
         <f t="shared" si="0"/>
-        <v>57.723994000000005</v>
+        <v>80.470962</v>
       </c>
       <c r="C22" s="3">
         <v>48.62</v>

</xml_diff>

<commit_message>
master: added test video and logs
</commit_message>
<xml_diff>
--- a/docs/project_management/time_estimation/time_estimation.xlsx
+++ b/docs/project_management/time_estimation/time_estimation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D070497\OneDrive - SAP SE\Workspaces\IdeaProjects\dashup\docs\project_management\time_estimation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="8_{38D201AD-A7A5-43E4-9BB3-0ED51C1379B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{957040BF-1B48-433F-A203-EEB4A582B69C}"/>
+  <xr:revisionPtr revIDLastSave="83" documentId="8_{38D201AD-A7A5-43E4-9BB3-0ED51C1379B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{0014DA0E-2835-4063-A182-8D17ED1E0026}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" xr2:uid="{70860DB2-D251-46E3-A3E4-9E8731226EC1}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Time Estimation</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Estimated Time In Hours</t>
+  </si>
+  <si>
+    <t>Actual Time in Hours</t>
   </si>
 </sst>
 </file>
@@ -359,28 +362,28 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$B$8</c:f>
+              <c:f>Sheet1!$C$5:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>12.54</c:v>
+                  <c:v>35.54</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41.71</c:v>
+                  <c:v>92.08</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.61</c:v>
+                  <c:v>46.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.39</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$5:$C$8</c:f>
+              <c:f>Sheet1!$B$5:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1274,14 +1277,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>6832</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>261937</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>83032</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1606,17 +1609,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88474A7B-6DD3-422E-8062-2B1A433E6E68}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="B4" sqref="B4:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.88671875" customWidth="1"/>
     <col min="2" max="2" width="23.109375" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
@@ -1626,106 +1630,117 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2">
-        <v>12.54</v>
-      </c>
-      <c r="C5" s="3">
+      <c r="B5" s="3">
         <v>16.72</v>
+      </c>
+      <c r="C5" s="2">
+        <v>35.54</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="2">
-        <v>41.71</v>
-      </c>
-      <c r="C6" s="3">
+      <c r="B6" s="3">
         <v>55.59</v>
+      </c>
+      <c r="C6" s="2">
+        <v>92.08</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
-        <v>10.61</v>
-      </c>
-      <c r="C7" s="3">
+      <c r="B7" s="3">
         <v>59.84</v>
+      </c>
+      <c r="C7" s="2">
+        <v>46.75</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2">
-        <v>6.39</v>
-      </c>
-      <c r="C8" s="3">
+      <c r="B8" s="3">
         <v>36.06</v>
+      </c>
+      <c r="C8" s="2">
+        <v>9.5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="2"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="17" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>11</v>
       </c>
       <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>7</v>
       </c>
       <c r="B20" s="2">
-        <f>1.6551*C20</f>
+        <f>1.6551*D20</f>
         <v>77.160761999999991</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="2">
+        <v>168.66</v>
+      </c>
+      <c r="D20" s="3">
         <v>46.62</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>8</v>
       </c>
       <c r="B21" s="2">
-        <f t="shared" ref="B21:B22" si="0">1.6551*C21</f>
+        <f>1.6551*D21</f>
         <v>78.815861999999996</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="2">
+        <v>69.5</v>
+      </c>
+      <c r="D21" s="3">
         <v>47.62</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>4</v>
       </c>
       <c r="B22" s="2">
-        <f t="shared" si="0"/>
+        <f>1.6551*D22</f>
         <v>80.470962</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
+        <v>121</v>
+      </c>
+      <c r="D22" s="3">
         <v>48.62</v>
       </c>
     </row>

</xml_diff>

<commit_message>
master: added actual time spent in fp analysis
</commit_message>
<xml_diff>
--- a/docs/project_management/time_estimation/time_estimation.xlsx
+++ b/docs/project_management/time_estimation/time_estimation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D070497\OneDrive - SAP SE\Workspaces\IdeaProjects\dashup\docs\project_management\time_estimation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="8_{38D201AD-A7A5-43E4-9BB3-0ED51C1379B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{0014DA0E-2835-4063-A182-8D17ED1E0026}"/>
+  <xr:revisionPtr revIDLastSave="140" documentId="8_{38D201AD-A7A5-43E4-9BB3-0ED51C1379B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{B7EBDEF1-B601-4467-807B-18D30EBE577E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" xr2:uid="{70860DB2-D251-46E3-A3E4-9E8731226EC1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{70860DB2-D251-46E3-A3E4-9E8731226EC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Time Estimation</t>
   </si>
@@ -68,7 +68,10 @@
     <t>Estimated Time In Hours</t>
   </si>
   <si>
-    <t>Actual Time in Hours</t>
+    <t>Use Case</t>
+  </si>
+  <si>
+    <t>Actual Time In Hours</t>
   </si>
 </sst>
 </file>
@@ -218,7 +221,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -326,8 +329,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="5.3274278215223202E-2"/>
-                  <c:y val="-0.18262800149190386"/>
+                  <c:x val="0.1304524381135761"/>
+                  <c:y val="-0.37094684060014887"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -362,7 +365,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$5:$C$8</c:f>
+              <c:f>Sheet1!$B$4:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -370,20 +373,20 @@
                   <c:v>35.54</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>92.08</c:v>
+                  <c:v>116.08</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>46.75</c:v>
+                  <c:v>41.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.5</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$B$8</c:f>
+              <c:f>Sheet1!$C$4:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -406,6 +409,135 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-23B5-41F0-8509-85FE1621CC44}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Series2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$19:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>168.67</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>121</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$19:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>46.62</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>47.62</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>48.62</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5279-4DD8-A79D-047707315EFB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -463,7 +595,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Estimated Time In Hours</a:t>
+                  <a:t>Time Spent In Hours</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -583,13 +715,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Function</a:t>
+                  <a:t>Function Points</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Points</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1276,15 +1403,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>6832</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>83032</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1609,138 +1736,158 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88474A7B-6DD3-422E-8062-2B1A433E6E68}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B8"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.88671875" customWidth="1"/>
-    <col min="2" max="2" width="23.109375" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>35.54</v>
+      </c>
+      <c r="C4" s="3">
+        <v>16.72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="3">
-        <v>16.72</v>
-      </c>
-      <c r="C5" s="2">
-        <v>35.54</v>
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>116.08</v>
+      </c>
+      <c r="C5" s="3">
+        <v>55.59</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="3">
-        <v>55.59</v>
-      </c>
-      <c r="C6" s="2">
-        <v>92.08</v>
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>41.25</v>
+      </c>
+      <c r="C6" s="3">
+        <v>59.84</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3">
-        <v>59.84</v>
-      </c>
-      <c r="C7" s="2">
-        <v>46.75</v>
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>23</v>
+      </c>
+      <c r="C7" s="3">
+        <v>36.06</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3">
-        <v>36.06</v>
-      </c>
-      <c r="C8" s="2">
-        <v>9.5</v>
-      </c>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="17" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A17" s="1" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="2"/>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
+      <c r="C12" s="3"/>
+    </row>
+    <row r="16" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="C18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="2">
+        <f>1.2538*D19</f>
+        <v>58.452155999999995</v>
+      </c>
+      <c r="C19" s="2">
+        <v>168.67</v>
+      </c>
+      <c r="D19" s="3">
+        <v>46.62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B20" s="2">
-        <f>1.6551*D20</f>
-        <v>77.160761999999991</v>
+        <f>1.2538*D20</f>
+        <v>59.705956</v>
       </c>
       <c r="C20" s="2">
-        <v>168.66</v>
+        <v>72.5</v>
       </c>
       <c r="D20" s="3">
-        <v>46.62</v>
+        <v>47.62</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B21" s="2">
-        <f>1.6551*D21</f>
-        <v>78.815861999999996</v>
+        <f>1.2538*D21</f>
+        <v>60.959755999999999</v>
       </c>
       <c r="C21" s="2">
-        <v>69.5</v>
+        <v>121</v>
       </c>
       <c r="D21" s="3">
-        <v>47.62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="2">
-        <f>1.6551*D22</f>
-        <v>80.470962</v>
-      </c>
-      <c r="C22" s="2">
-        <v>121</v>
-      </c>
-      <c r="D22" s="3">
         <v>48.62</v>
       </c>
     </row>

</xml_diff>